<commit_message>
Update dictionaries after last Ivy engagement
</commit_message>
<xml_diff>
--- a/data dictionaries/SFC_Data_Dictionary.xlsx
+++ b/data dictionaries/SFC_Data_Dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjectCollections\Programs\Australia_Cultural_Data_Engine\data_management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EAFA4D7-0690-4CB0-B1DA-BB88564C7795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBFEDFB0-D60A-416B-AE29-AD6CF3B5D22E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="99">
   <si>
     <t xml:space="preserve"> System control number (NR)</t>
   </si>
@@ -60,12 +60,6 @@
     <t xml:space="preserve"> Title_10</t>
   </si>
   <si>
-    <t xml:space="preserve"> Place of publication, distribution</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Date of publication, distribution</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Physical Description</t>
   </si>
   <si>
@@ -243,9 +237,6 @@
     <t>rename as "note"</t>
   </si>
   <si>
-    <t>rename as "date_info.date_created"</t>
-  </si>
-  <si>
     <t>rename as "title"</t>
   </si>
   <si>
@@ -322,6 +313,15 @@
   </si>
   <si>
     <t>Newly construct _class_ori = "resource"</t>
+  </si>
+  <si>
+    <t>It seems that this is another property of date.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Date of publication</t>
+  </si>
+  <si>
+    <t>rename as "date_info.date_published.raw_txt"</t>
   </si>
 </sst>
 </file>
@@ -690,150 +690,150 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="4"/>
-    <col min="2" max="2" width="8.88671875" style="4" customWidth="1"/>
-    <col min="3" max="4" width="8.88671875" style="4"/>
-    <col min="5" max="5" width="40.5546875" style="11" customWidth="1"/>
-    <col min="6" max="6" width="34.77734375" style="11" customWidth="1"/>
-    <col min="7" max="7" width="35.5546875" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="4"/>
+    <col min="1" max="1" width="8.85546875" style="4"/>
+    <col min="2" max="2" width="8.85546875" style="4" customWidth="1"/>
+    <col min="3" max="4" width="8.85546875" style="4"/>
+    <col min="5" max="5" width="40.5703125" style="11" customWidth="1"/>
+    <col min="6" max="6" width="34.7109375" style="11" customWidth="1"/>
+    <col min="7" max="7" width="35.5703125" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="G1" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G2" s="7"/>
     </row>
-    <row r="3" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B3" s="6">
         <v>1</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G3" s="7"/>
     </row>
-    <row r="4" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B4" s="6">
         <v>2</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G4" s="7"/>
     </row>
-    <row r="5" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B5" s="6">
         <v>3</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G5" s="7"/>
     </row>
-    <row r="6" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B6" s="6">
         <v>4</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>4</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G6" s="7"/>
     </row>
-    <row r="7" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>100</v>
       </c>
@@ -841,22 +841,22 @@
         <v>1</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>245</v>
       </c>
@@ -864,20 +864,20 @@
         <v>0</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>5</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G8" s="7"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>245</v>
       </c>
@@ -888,17 +888,17 @@
         <v>0</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>6</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>245</v>
       </c>
@@ -909,17 +909,17 @@
         <v>2</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>7</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G10" s="7"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>245</v>
       </c>
@@ -930,17 +930,17 @@
         <v>3</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>245</v>
       </c>
@@ -951,17 +951,17 @@
         <v>4</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>9</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>245</v>
       </c>
@@ -972,122 +972,124 @@
         <v>0</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>10</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>260</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>11</v>
+        <v>82</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="G14" s="7"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>260</v>
       </c>
       <c r="B15" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>35</v>
-      </c>
       <c r="E15" s="7" t="s">
-        <v>12</v>
+        <v>97</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>72</v>
+        <v>98</v>
       </c>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>300</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G16" s="7"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>500</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G17" s="7"/>
     </row>
-    <row r="18" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>506</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G18" s="7"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>520</v>
       </c>
@@ -1095,41 +1097,41 @@
         <v>2</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G19" s="7"/>
     </row>
-    <row r="20" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>541</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G20" s="7"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>545</v>
       </c>
@@ -1137,83 +1139,83 @@
         <v>0</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G21" s="7"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>590</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G22" s="7"/>
     </row>
-    <row r="23" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>595</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G23" s="7"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>599</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G24" s="7"/>
     </row>
-    <row r="25" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>700</v>
       </c>
@@ -1221,20 +1223,20 @@
         <v>1</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G25" s="7"/>
     </row>
-    <row r="26" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>710</v>
       </c>
@@ -1242,359 +1244,359 @@
         <v>2</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>787</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G27" s="7"/>
     </row>
-    <row r="28" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>852</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D28" s="8">
         <v>3</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G28" s="7"/>
     </row>
-    <row r="29" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>852</v>
       </c>
       <c r="B29" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C29" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>35</v>
-      </c>
       <c r="E29" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G29" s="7"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>852</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G30" s="7"/>
     </row>
-    <row r="31" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>852</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G31" s="7"/>
     </row>
-    <row r="32" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>852</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G32" s="7"/>
     </row>
-    <row r="33" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>856</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G33" s="7"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>900</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G34" s="7"/>
     </row>
-    <row r="35" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>900</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G35" s="7"/>
     </row>
-    <row r="36" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>910</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G36" s="7"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>920</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G37" s="7"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>930</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G38" s="7"/>
     </row>
-    <row r="39" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>942</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G39" s="7"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E40" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G40" s="7"/>
+    </row>
+    <row r="41" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="F40" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="G40" s="7"/>
-    </row>
-    <row r="41" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A41" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="E41" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="G41" s="7" t="s">
+      <c r="E43" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G43" s="10"/>
+    </row>
+    <row r="44" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="F44" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F45" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="F46" s="11" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="E42" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="F42" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="G42" s="7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="E43" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="G43" s="10"/>
-    </row>
-    <row r="44" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="F44" s="11" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F45" s="11" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="F46" s="11" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>